<commit_message>
73782-adding a column to display figures after 10 months
</commit_message>
<xml_diff>
--- a/src/ESFA.DC.ILR.ReportService.Service/Reports/Templates/AdultFundingClaimReportTemplate.xlsx
+++ b/src/ESFA.DC.ILR.ReportService.Service/Reports/Templates/AdultFundingClaimReportTemplate.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21425"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5B297C4-5F23-42E6-A40C-6C12244D2C16}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3DA6C40-1390-4E2F-B485-BF3BD1F69D78}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Adult Funding Claim" sheetId="3" r:id="rId1"/>
@@ -13,13 +13,13 @@
   <definedNames>
     <definedName name="_xlnm.Print_Area" localSheetId="0">'Adult Funding Claim'!$B$2:$H$41</definedName>
   </definedNames>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <fileRecoveryPr autoRecover="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="29">
   <si>
     <t>Provider :</t>
   </si>
@@ -121,8 +121,13 @@
   </si>
   <si>
     <t>Actual earnings 
+(10 months)
+- year-end claims</t>
+  </si>
+  <si>
+    <t>Actual earnings 
 (12 months)
-- year-end and final-year claims</t>
+- final-year claims</t>
   </si>
 </sst>
 </file>
@@ -130,8 +135,8 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="4">
-    <numFmt numFmtId="8" formatCode="&quot;£&quot;#,##0.00;[Red]\-&quot;£&quot;#,##0.00"/>
-    <numFmt numFmtId="164" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="164" formatCode="&quot;£&quot;#,##0.00;[Red]\-&quot;£&quot;#,##0.00"/>
     <numFmt numFmtId="165" formatCode="_-[$£-809]* #,##0.00_-;\-[$£-809]* #,##0.00_-;_-[$£-809]* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="166" formatCode="&quot;£&quot;#,##0.00"/>
   </numFmts>
@@ -373,10 +378,10 @@
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="57">
+  <cellXfs count="54">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -389,7 +394,6 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="5" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="5" xfId="2" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
@@ -408,7 +412,7 @@
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="6" xfId="2" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="8" fontId="3" fillId="2" borderId="7" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="164" fontId="3" fillId="2" borderId="7" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="top" wrapText="1"/>
       <protection locked="0"/>
     </xf>
@@ -443,12 +447,6 @@
       <alignment horizontal="right" vertical="top" wrapText="1" readingOrder="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
@@ -456,9 +454,6 @@
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="9" xfId="2" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -481,6 +476,51 @@
       <alignment horizontal="center" vertical="top" wrapText="1" readingOrder="1"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="10" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="top" wrapText="1" readingOrder="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="12" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="top" wrapText="1" readingOrder="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="11" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="top" wrapText="1" readingOrder="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="10" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="12" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="11" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="10" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="12" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="11" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="8" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="6" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="10" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="top" wrapText="1" readingOrder="1"/>
       <protection locked="0"/>
@@ -493,53 +533,13 @@
       <alignment vertical="top" wrapText="1" readingOrder="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="10" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="top" wrapText="1" readingOrder="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="12" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="top" wrapText="1" readingOrder="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="11" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="top" wrapText="1" readingOrder="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="10" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="12" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="11" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="10" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="12" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="11" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="8" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="6" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="5" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right" vertical="top" wrapText="1" readingOrder="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="5" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right" vertical="top" wrapText="1" readingOrder="1"/>
+      <protection locked="0"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -635,9 +635,9 @@
       <xdr:col>1</xdr:col>
       <xdr:colOff>314324</xdr:colOff>
       <xdr:row>27</xdr:row>
-      <xdr:rowOff>57149</xdr:rowOff>
+      <xdr:rowOff>4756</xdr:rowOff>
     </xdr:from>
-    <xdr:ext cx="7038975" cy="1066801"/>
+    <xdr:ext cx="7839076" cy="1066801"/>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
         <xdr:cNvPr id="2" name="TextBox 1">
@@ -651,8 +651,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="538162" y="8710612"/>
-          <a:ext cx="7038975" cy="1066801"/>
+          <a:off x="523874" y="5681656"/>
+          <a:ext cx="7839076" cy="1066801"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1163,8 +1163,8 @@
   </sheetPr>
   <dimension ref="B2:I41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B40" sqref="B40:D40"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="M11" sqref="M11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1173,11 +1173,11 @@
     <col min="2" max="2" width="5.7109375" style="4" customWidth="1"/>
     <col min="3" max="3" width="18.28515625" style="4" customWidth="1"/>
     <col min="4" max="4" width="22.85546875" style="4" customWidth="1"/>
-    <col min="5" max="5" width="18.85546875" style="4" customWidth="1"/>
-    <col min="6" max="7" width="20.7109375" style="4" customWidth="1"/>
-    <col min="8" max="8" width="6.28515625" style="4" customWidth="1"/>
-    <col min="9" max="9" width="2.28515625" style="4" customWidth="1"/>
-    <col min="10" max="16384" width="9.140625" style="4"/>
+    <col min="5" max="5" width="13" style="4" customWidth="1"/>
+    <col min="6" max="8" width="20.7109375" style="4" customWidth="1"/>
+    <col min="9" max="9" width="6.28515625" style="4" customWidth="1"/>
+    <col min="10" max="10" width="2.28515625" style="4" customWidth="1"/>
+    <col min="11" max="16384" width="9.140625" style="4"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:9" x14ac:dyDescent="0.2">
@@ -1187,7 +1187,8 @@
       <c r="E2" s="2"/>
       <c r="F2" s="2"/>
       <c r="G2" s="2"/>
-      <c r="H2" s="3"/>
+      <c r="H2" s="2"/>
+      <c r="I2" s="3"/>
     </row>
     <row r="3" spans="2:9" ht="20.25" x14ac:dyDescent="0.2">
       <c r="B3" s="5"/>
@@ -1196,348 +1197,384 @@
       </c>
       <c r="D3" s="7"/>
       <c r="E3" s="7"/>
-      <c r="F3" s="42" t="s">
+      <c r="G3" s="35"/>
+      <c r="H3" s="35" t="s">
         <v>10</v>
       </c>
-      <c r="G3" s="42"/>
-      <c r="H3" s="8"/>
-      <c r="I3" s="9"/>
+      <c r="I3" s="8"/>
     </row>
     <row r="4" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B4" s="5"/>
-      <c r="C4" s="10"/>
-      <c r="D4" s="10"/>
-      <c r="E4" s="10"/>
-      <c r="F4" s="10"/>
-      <c r="G4" s="10"/>
-      <c r="H4" s="11"/>
+      <c r="C4" s="9"/>
+      <c r="D4" s="9"/>
+      <c r="E4" s="9"/>
+      <c r="F4" s="7"/>
+      <c r="G4" s="7"/>
+      <c r="H4" s="9"/>
+      <c r="I4" s="10"/>
     </row>
     <row r="5" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B5" s="5"/>
-      <c r="C5" s="12" t="s">
+      <c r="C5" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="D5" s="13"/>
-      <c r="E5" s="13"/>
-      <c r="F5" s="10"/>
+      <c r="D5" s="12"/>
+      <c r="E5" s="12"/>
+      <c r="F5" s="7"/>
       <c r="G5" s="7"/>
-      <c r="H5" s="8"/>
-      <c r="I5" s="9"/>
+      <c r="H5" s="7"/>
+      <c r="I5" s="8"/>
     </row>
     <row r="6" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B6" s="5"/>
-      <c r="C6" s="12" t="s">
+      <c r="C6" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="D6" s="14"/>
-      <c r="E6" s="14"/>
-      <c r="F6" s="10"/>
+      <c r="D6" s="13"/>
+      <c r="E6" s="13"/>
+      <c r="F6" s="7"/>
       <c r="G6" s="7"/>
-      <c r="H6" s="8"/>
-      <c r="I6" s="9"/>
+      <c r="H6" s="7"/>
+      <c r="I6" s="8"/>
     </row>
     <row r="7" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B7" s="5"/>
-      <c r="C7" s="12" t="s">
+      <c r="C7" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="D7" s="15"/>
-      <c r="E7" s="15"/>
-      <c r="F7" s="35"/>
-      <c r="G7" s="36" t="s">
+      <c r="D7" s="14"/>
+      <c r="E7" s="14"/>
+      <c r="F7" s="31"/>
+      <c r="H7" s="32" t="s">
         <v>25</v>
       </c>
-      <c r="H7" s="8"/>
-      <c r="I7" s="9"/>
+      <c r="I7" s="8"/>
     </row>
     <row r="8" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B8" s="5"/>
-      <c r="C8" s="16"/>
-      <c r="D8" s="16"/>
-      <c r="E8" s="16"/>
-      <c r="F8" s="16"/>
-      <c r="G8" s="16"/>
-      <c r="H8" s="11"/>
+      <c r="C8" s="15"/>
+      <c r="D8" s="15"/>
+      <c r="E8" s="15"/>
+      <c r="F8" s="15"/>
+      <c r="G8" s="15"/>
+      <c r="H8" s="15"/>
+      <c r="I8" s="10"/>
     </row>
     <row r="9" spans="2:9" ht="28.9" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B9" s="5"/>
-      <c r="C9" s="46" t="s">
+      <c r="C9" s="40" t="s">
         <v>24</v>
       </c>
-      <c r="D9" s="46"/>
-      <c r="E9" s="46"/>
-      <c r="F9" s="46"/>
-      <c r="G9" s="46"/>
-      <c r="H9" s="11"/>
+      <c r="D9" s="40"/>
+      <c r="E9" s="40"/>
+      <c r="F9" s="40"/>
+      <c r="G9" s="40"/>
+      <c r="H9" s="15"/>
+      <c r="I9" s="10"/>
     </row>
     <row r="10" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B10" s="5"/>
-      <c r="C10" s="10"/>
-      <c r="D10" s="10"/>
-      <c r="E10" s="10"/>
-      <c r="F10" s="10"/>
-      <c r="G10" s="10"/>
-      <c r="H10" s="11"/>
+      <c r="C10" s="9"/>
+      <c r="D10" s="9"/>
+      <c r="E10" s="9"/>
+      <c r="F10" s="9"/>
+      <c r="G10" s="9"/>
+      <c r="H10" s="9"/>
+      <c r="I10" s="10"/>
     </row>
     <row r="11" spans="2:9" ht="51" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B11" s="5"/>
-      <c r="C11" s="50" t="s">
+      <c r="C11" s="44" t="s">
         <v>20</v>
       </c>
-      <c r="D11" s="51"/>
-      <c r="E11" s="52"/>
-      <c r="F11" s="37" t="s">
+      <c r="D11" s="45"/>
+      <c r="E11" s="46"/>
+      <c r="F11" s="33" t="s">
         <v>26</v>
       </c>
-      <c r="G11" s="37" t="s">
+      <c r="G11" s="33" t="s">
         <v>27</v>
       </c>
-      <c r="H11" s="11"/>
+      <c r="H11" s="33" t="s">
+        <v>28</v>
+      </c>
+      <c r="I11" s="10"/>
     </row>
     <row r="12" spans="2:9" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B12" s="5"/>
-      <c r="C12" s="43" t="s">
+      <c r="C12" s="37" t="s">
         <v>22</v>
       </c>
-      <c r="D12" s="44"/>
-      <c r="E12" s="45"/>
-      <c r="F12" s="17"/>
-      <c r="G12" s="17"/>
-      <c r="H12" s="11"/>
+      <c r="D12" s="38"/>
+      <c r="E12" s="39"/>
+      <c r="F12" s="16"/>
+      <c r="G12" s="16"/>
+      <c r="H12" s="16"/>
+      <c r="I12" s="10"/>
     </row>
     <row r="13" spans="2:9" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B13" s="5"/>
-      <c r="C13" s="43" t="s">
+      <c r="C13" s="37" t="s">
         <v>23</v>
       </c>
-      <c r="D13" s="44"/>
-      <c r="E13" s="45"/>
-      <c r="F13" s="17"/>
-      <c r="G13" s="17"/>
-      <c r="H13" s="11"/>
+      <c r="D13" s="38"/>
+      <c r="E13" s="39"/>
+      <c r="F13" s="16"/>
+      <c r="G13" s="16"/>
+      <c r="H13" s="16"/>
+      <c r="I13" s="10"/>
     </row>
     <row r="14" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B14" s="5"/>
-      <c r="C14" s="43" t="s">
+      <c r="C14" s="37" t="s">
         <v>7</v>
       </c>
-      <c r="D14" s="44"/>
-      <c r="E14" s="45"/>
-      <c r="F14" s="17"/>
-      <c r="G14" s="17"/>
-      <c r="H14" s="11"/>
+      <c r="D14" s="38"/>
+      <c r="E14" s="39"/>
+      <c r="F14" s="16"/>
+      <c r="G14" s="16"/>
+      <c r="H14" s="16"/>
+      <c r="I14" s="10"/>
     </row>
     <row r="15" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B15" s="5"/>
-      <c r="C15" s="43" t="s">
+      <c r="C15" s="37" t="s">
         <v>8</v>
       </c>
-      <c r="D15" s="44"/>
-      <c r="E15" s="45"/>
-      <c r="F15" s="17"/>
-      <c r="G15" s="17"/>
-      <c r="H15" s="11"/>
+      <c r="D15" s="38"/>
+      <c r="E15" s="39"/>
+      <c r="F15" s="16"/>
+      <c r="G15" s="16"/>
+      <c r="H15" s="16"/>
+      <c r="I15" s="10"/>
     </row>
     <row r="16" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B16" s="5"/>
-      <c r="C16" s="43" t="s">
+      <c r="C16" s="37" t="s">
         <v>9</v>
       </c>
-      <c r="D16" s="44"/>
-      <c r="E16" s="45"/>
-      <c r="F16" s="17"/>
-      <c r="G16" s="17"/>
-      <c r="H16" s="11"/>
-    </row>
-    <row r="17" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="D16" s="38"/>
+      <c r="E16" s="39"/>
+      <c r="F16" s="16"/>
+      <c r="G16" s="16"/>
+      <c r="H16" s="16"/>
+      <c r="I16" s="10"/>
+    </row>
+    <row r="17" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B17" s="5"/>
-      <c r="C17" s="33"/>
-      <c r="D17" s="34"/>
-      <c r="E17" s="34"/>
-      <c r="F17" s="19"/>
-      <c r="G17" s="20"/>
-      <c r="H17" s="11"/>
-    </row>
-    <row r="18" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="C17" s="29"/>
+      <c r="D17" s="30"/>
+      <c r="E17" s="30"/>
+      <c r="F17" s="18"/>
+      <c r="G17" s="19"/>
+      <c r="H17" s="52"/>
+      <c r="I17" s="10"/>
+    </row>
+    <row r="18" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B18" s="5"/>
-      <c r="C18" s="43" t="s">
+      <c r="C18" s="37" t="s">
         <v>21</v>
       </c>
-      <c r="D18" s="44"/>
-      <c r="E18" s="45"/>
-      <c r="F18" s="21">
+      <c r="D18" s="38"/>
+      <c r="E18" s="39"/>
+      <c r="F18" s="20">
         <f>SUM(F12:F16)</f>
         <v>0</v>
       </c>
-      <c r="G18" s="21">
+      <c r="G18" s="20">
         <f>SUM(G12:G16)</f>
         <v>0</v>
       </c>
-      <c r="H18" s="11"/>
-    </row>
-    <row r="19" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="H18" s="20">
+        <f>SUM(H12:H16)</f>
+        <v>0</v>
+      </c>
+      <c r="I18" s="10"/>
+    </row>
+    <row r="19" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B19" s="5"/>
-      <c r="C19" s="10"/>
-      <c r="D19" s="10"/>
-      <c r="E19" s="10"/>
-      <c r="F19" s="10"/>
-      <c r="G19" s="10"/>
-      <c r="H19" s="11"/>
-    </row>
-    <row r="20" spans="2:8" ht="54" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C19" s="9"/>
+      <c r="D19" s="9"/>
+      <c r="E19" s="9"/>
+      <c r="F19" s="9"/>
+      <c r="G19" s="9"/>
+      <c r="H19" s="10"/>
+      <c r="I19" s="10"/>
+    </row>
+    <row r="20" spans="2:9" ht="54" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B20" s="5"/>
-      <c r="C20" s="47" t="s">
+      <c r="C20" s="41" t="s">
         <v>18</v>
       </c>
-      <c r="D20" s="48"/>
-      <c r="E20" s="49"/>
-      <c r="F20" s="38" t="s">
+      <c r="D20" s="42"/>
+      <c r="E20" s="43"/>
+      <c r="F20" s="34" t="s">
         <v>26</v>
       </c>
-      <c r="G20" s="38" t="s">
+      <c r="G20" s="33" t="s">
         <v>27</v>
       </c>
-      <c r="H20" s="11"/>
-    </row>
-    <row r="21" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="H20" s="33" t="s">
+        <v>28</v>
+      </c>
+      <c r="I20" s="10"/>
+    </row>
+    <row r="21" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B21" s="5"/>
-      <c r="C21" s="39" t="s">
+      <c r="C21" s="49" t="s">
         <v>3</v>
       </c>
-      <c r="D21" s="40"/>
-      <c r="E21" s="41"/>
-      <c r="F21" s="22"/>
-      <c r="G21" s="22"/>
-      <c r="H21" s="11"/>
-    </row>
-    <row r="22" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="D21" s="50"/>
+      <c r="E21" s="51"/>
+      <c r="F21" s="21"/>
+      <c r="G21" s="21"/>
+      <c r="H21" s="21"/>
+      <c r="I21" s="10"/>
+    </row>
+    <row r="22" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B22" s="5"/>
-      <c r="C22" s="39" t="s">
+      <c r="C22" s="49" t="s">
         <v>4</v>
       </c>
-      <c r="D22" s="40"/>
-      <c r="E22" s="41"/>
-      <c r="F22" s="22"/>
-      <c r="G22" s="22"/>
-      <c r="H22" s="11"/>
-    </row>
-    <row r="23" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="D22" s="50"/>
+      <c r="E22" s="51"/>
+      <c r="F22" s="21"/>
+      <c r="G22" s="21"/>
+      <c r="H22" s="21"/>
+      <c r="I22" s="10"/>
+    </row>
+    <row r="23" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B23" s="5"/>
-      <c r="C23" s="39" t="s">
+      <c r="C23" s="49" t="s">
         <v>5</v>
       </c>
-      <c r="D23" s="40"/>
-      <c r="E23" s="41"/>
-      <c r="F23" s="22"/>
-      <c r="G23" s="22"/>
-      <c r="H23" s="11"/>
-    </row>
-    <row r="24" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="D23" s="50"/>
+      <c r="E23" s="51"/>
+      <c r="F23" s="21"/>
+      <c r="G23" s="21"/>
+      <c r="H23" s="21"/>
+      <c r="I23" s="10"/>
+    </row>
+    <row r="24" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B24" s="5"/>
-      <c r="C24" s="18"/>
-      <c r="D24" s="23"/>
-      <c r="E24" s="23"/>
-      <c r="F24" s="24"/>
-      <c r="G24" s="25"/>
-      <c r="H24" s="11"/>
-    </row>
-    <row r="25" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="C24" s="17"/>
+      <c r="D24" s="22"/>
+      <c r="E24" s="22"/>
+      <c r="F24" s="23"/>
+      <c r="G24" s="24"/>
+      <c r="H24" s="53"/>
+      <c r="I24" s="10"/>
+    </row>
+    <row r="25" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B25" s="5"/>
-      <c r="C25" s="39" t="s">
+      <c r="C25" s="49" t="s">
         <v>6</v>
       </c>
-      <c r="D25" s="40"/>
-      <c r="E25" s="41"/>
-      <c r="F25" s="21">
+      <c r="D25" s="50"/>
+      <c r="E25" s="51"/>
+      <c r="F25" s="20">
         <f>SUM(F21:F23)</f>
         <v>0</v>
       </c>
-      <c r="G25" s="21">
+      <c r="G25" s="20">
         <f>SUM(G21:G23)</f>
         <v>0</v>
       </c>
-      <c r="H25" s="11"/>
-    </row>
-    <row r="26" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="H25" s="20">
+        <f>SUM(H21:H23)</f>
+        <v>0</v>
+      </c>
+      <c r="I25" s="10"/>
+    </row>
+    <row r="26" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B26" s="5"/>
-      <c r="C26" s="16"/>
-      <c r="D26" s="16"/>
-      <c r="E26" s="16"/>
-      <c r="F26" s="16"/>
-      <c r="G26" s="16"/>
-      <c r="H26" s="11"/>
-    </row>
-    <row r="27" spans="2:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C26" s="15"/>
+      <c r="D26" s="15"/>
+      <c r="E26" s="15"/>
+      <c r="F26" s="15"/>
+      <c r="G26" s="15"/>
+      <c r="H26" s="9"/>
+      <c r="I26" s="10"/>
+    </row>
+    <row r="27" spans="2:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B27" s="5"/>
-      <c r="C27" s="10"/>
-      <c r="D27" s="10"/>
-      <c r="E27" s="10"/>
-      <c r="F27" s="10"/>
-      <c r="G27" s="10"/>
-      <c r="H27" s="11"/>
-    </row>
-    <row r="28" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="C27" s="9"/>
+      <c r="D27" s="9"/>
+      <c r="E27" s="9"/>
+      <c r="F27" s="9"/>
+      <c r="G27" s="9"/>
+      <c r="H27" s="2"/>
+      <c r="I27" s="10"/>
+    </row>
+    <row r="28" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B28" s="5"/>
-      <c r="C28" s="10"/>
-      <c r="D28" s="10"/>
-      <c r="E28" s="10"/>
-      <c r="F28" s="10"/>
-      <c r="G28" s="10"/>
-      <c r="H28" s="11"/>
-    </row>
-    <row r="29" spans="2:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C28" s="9"/>
+      <c r="D28" s="9"/>
+      <c r="E28" s="9"/>
+      <c r="F28" s="9"/>
+      <c r="G28" s="9"/>
+      <c r="H28" s="9"/>
+      <c r="I28" s="10"/>
+    </row>
+    <row r="29" spans="2:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B29" s="5"/>
-      <c r="C29" s="10"/>
-      <c r="D29" s="10"/>
-      <c r="E29" s="10"/>
-      <c r="F29" s="10"/>
-      <c r="G29" s="10"/>
-      <c r="H29" s="11"/>
-    </row>
-    <row r="30" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="C29" s="9"/>
+      <c r="D29" s="9"/>
+      <c r="E29" s="9"/>
+      <c r="F29" s="9"/>
+      <c r="G29" s="9"/>
+      <c r="H29" s="9"/>
+      <c r="I29" s="10"/>
+    </row>
+    <row r="30" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B30" s="5"/>
-      <c r="C30" s="10"/>
-      <c r="D30" s="10"/>
-      <c r="E30" s="10"/>
-      <c r="F30" s="10"/>
-      <c r="G30" s="10"/>
-      <c r="H30" s="11"/>
-    </row>
-    <row r="31" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="C30" s="9"/>
+      <c r="D30" s="9"/>
+      <c r="E30" s="9"/>
+      <c r="F30" s="9"/>
+      <c r="G30" s="9"/>
+      <c r="H30" s="9"/>
+      <c r="I30" s="10"/>
+    </row>
+    <row r="31" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B31" s="5"/>
-      <c r="C31" s="10"/>
-      <c r="D31" s="10"/>
-      <c r="E31" s="10"/>
-      <c r="F31" s="10"/>
-      <c r="G31" s="10"/>
-      <c r="H31" s="11"/>
-    </row>
-    <row r="32" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="C31" s="9"/>
+      <c r="D31" s="9"/>
+      <c r="E31" s="9"/>
+      <c r="F31" s="9"/>
+      <c r="G31" s="9"/>
+      <c r="H31" s="9"/>
+      <c r="I31" s="10"/>
+    </row>
+    <row r="32" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B32" s="5"/>
-      <c r="C32" s="10"/>
-      <c r="D32" s="10"/>
-      <c r="E32" s="10"/>
-      <c r="F32" s="10"/>
-      <c r="G32" s="10"/>
-      <c r="H32" s="11"/>
+      <c r="C32" s="9"/>
+      <c r="D32" s="9"/>
+      <c r="E32" s="9"/>
+      <c r="F32" s="9"/>
+      <c r="G32" s="9"/>
+      <c r="H32" s="9"/>
+      <c r="I32" s="10"/>
     </row>
     <row r="33" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B33" s="5"/>
-      <c r="C33" s="10"/>
-      <c r="D33" s="10"/>
-      <c r="E33" s="10"/>
-      <c r="F33" s="10"/>
-      <c r="G33" s="10"/>
-      <c r="H33" s="11"/>
+      <c r="C33" s="9"/>
+      <c r="D33" s="9"/>
+      <c r="E33" s="9"/>
+      <c r="F33" s="9"/>
+      <c r="G33" s="9"/>
+      <c r="H33" s="9"/>
+      <c r="I33" s="10"/>
     </row>
     <row r="34" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B34" s="5"/>
-      <c r="C34" s="10"/>
-      <c r="D34" s="10"/>
-      <c r="E34" s="10"/>
-      <c r="F34" s="10"/>
-      <c r="G34" s="10"/>
-      <c r="H34" s="11"/>
+      <c r="C34" s="9"/>
+      <c r="D34" s="9"/>
+      <c r="E34" s="9"/>
+      <c r="F34" s="9"/>
+      <c r="G34" s="9"/>
+      <c r="H34" s="9"/>
+      <c r="I34" s="10"/>
     </row>
     <row r="35" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B35" s="5"/>
@@ -1546,80 +1583,88 @@
       <c r="E35" s="2"/>
       <c r="F35" s="2"/>
       <c r="G35" s="2"/>
-      <c r="H35" s="11"/>
+      <c r="H35" s="2"/>
+      <c r="I35" s="10"/>
     </row>
     <row r="36" spans="2:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B36" s="26" t="s">
+      <c r="B36" s="5"/>
+      <c r="C36" s="36" t="s">
         <v>11</v>
       </c>
-      <c r="C36" s="27"/>
-      <c r="D36" s="27"/>
-      <c r="E36" s="27" t="s">
+      <c r="D36" s="36"/>
+      <c r="E36" s="36"/>
+      <c r="F36" s="36" t="s">
         <v>12</v>
       </c>
-      <c r="F36" s="27"/>
-      <c r="H36" s="28"/>
+      <c r="G36" s="36"/>
+      <c r="I36" s="10"/>
     </row>
     <row r="37" spans="2:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B37" s="26" t="s">
+      <c r="B37" s="5"/>
+      <c r="C37" s="36" t="s">
         <v>14</v>
       </c>
-      <c r="C37" s="27"/>
-      <c r="D37" s="27"/>
-      <c r="E37" s="27" t="s">
+      <c r="D37" s="36"/>
+      <c r="E37" s="36"/>
+      <c r="F37" s="36" t="s">
         <v>13</v>
       </c>
-      <c r="F37" s="27"/>
-      <c r="H37" s="28"/>
+      <c r="G37" s="36"/>
+      <c r="I37" s="10"/>
     </row>
     <row r="38" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B38" s="26" t="s">
+      <c r="B38" s="5"/>
+      <c r="C38" s="36" t="s">
         <v>17</v>
       </c>
-      <c r="C38" s="27"/>
-      <c r="D38" s="29"/>
-      <c r="E38" s="27" t="s">
+      <c r="D38" s="36"/>
+      <c r="E38" s="26"/>
+      <c r="F38" s="36" t="s">
         <v>15</v>
       </c>
-      <c r="F38" s="27"/>
-      <c r="G38" s="27"/>
-      <c r="H38" s="28"/>
-      <c r="I38" s="27"/>
+      <c r="G38" s="36"/>
+      <c r="H38" s="36"/>
+      <c r="I38" s="25"/>
     </row>
     <row r="39" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B39" s="26"/>
-      <c r="C39" s="27"/>
-      <c r="D39" s="27"/>
-      <c r="E39" s="27" t="s">
+      <c r="B39" s="5"/>
+      <c r="C39" s="36"/>
+      <c r="D39" s="36"/>
+      <c r="E39" s="36"/>
+      <c r="F39" s="36" t="s">
         <v>16</v>
       </c>
-      <c r="F39" s="27"/>
-      <c r="G39" s="27"/>
-      <c r="H39" s="28"/>
-      <c r="I39" s="27"/>
+      <c r="G39" s="36"/>
+      <c r="H39" s="36"/>
+      <c r="I39" s="25"/>
     </row>
     <row r="40" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B40" s="55"/>
-      <c r="C40" s="56"/>
-      <c r="D40" s="56"/>
-      <c r="E40" s="27"/>
-      <c r="F40" s="27"/>
-      <c r="G40" s="27"/>
-      <c r="H40" s="30"/>
-      <c r="I40" s="31"/>
+      <c r="B40" s="5"/>
+      <c r="C40" s="36"/>
+      <c r="D40" s="36"/>
+      <c r="E40" s="36"/>
+      <c r="F40" s="36"/>
+      <c r="G40" s="36"/>
+      <c r="H40" s="36"/>
+      <c r="I40" s="27"/>
     </row>
     <row r="41" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B41" s="53"/>
-      <c r="C41" s="54"/>
-      <c r="D41" s="54"/>
-      <c r="E41" s="16"/>
-      <c r="F41" s="16"/>
-      <c r="G41" s="16"/>
-      <c r="H41" s="32"/>
+      <c r="B41" s="47"/>
+      <c r="C41" s="48"/>
+      <c r="D41" s="48"/>
+      <c r="E41" s="15"/>
+      <c r="F41" s="15"/>
+      <c r="G41" s="15"/>
+      <c r="H41" s="15"/>
+      <c r="I41" s="28"/>
     </row>
   </sheetData>
-  <mergeCells count="16">
-    <mergeCell ref="F3:G3"/>
+  <mergeCells count="14">
+    <mergeCell ref="B41:D41"/>
+    <mergeCell ref="C21:E21"/>
+    <mergeCell ref="C22:E22"/>
+    <mergeCell ref="C23:E23"/>
+    <mergeCell ref="C25:E25"/>
     <mergeCell ref="C12:E12"/>
     <mergeCell ref="C13:E13"/>
     <mergeCell ref="C9:G9"/>
@@ -1629,15 +1674,9 @@
     <mergeCell ref="C15:E15"/>
     <mergeCell ref="C16:E16"/>
     <mergeCell ref="C18:E18"/>
-    <mergeCell ref="B41:D41"/>
-    <mergeCell ref="C21:E21"/>
-    <mergeCell ref="C22:E22"/>
-    <mergeCell ref="C23:E23"/>
-    <mergeCell ref="C25:E25"/>
-    <mergeCell ref="B40:D40"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" scale="78" orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="9" scale="73" orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>